<commit_message>
Atualização do simulador financeiro no Excel: Adição da aba 'melhorias' e upload do código da calculadora.
</commit_message>
<xml_diff>
--- a/GuilhermeToledo/SimuladorFinanceiro_v1.xlsx
+++ b/GuilhermeToledo/SimuladorFinanceiro_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - SPTech School\202501\Pesquisa e Inovação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_toledo_sptech_school/Documents/202501/Pesquisa e Inovação/repositorio_PI/GuilhermeToledo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF76DA37-AE53-42E6-AFF1-46FDB6BE44D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{EF76DA37-AE53-42E6-AFF1-46FDB6BE44D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EEDC959-B906-46A0-9A18-3E9E49DD7008}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EF024B9-F251-4A5D-B513-02DE12B0E257}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2EF024B9-F251-4A5D-B513-02DE12B0E257}"/>
   </bookViews>
   <sheets>
     <sheet name="calc v1" sheetId="1" r:id="rId1"/>
@@ -244,10 +244,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-[$R$-416]\ * #,##0.0000_-;\-[$R$-416]\ * #,##0.0000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_-[$R$-416]\ * #,##0.00000_-;\-[$R$-416]\ * #,##0.00000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.0000_-;\-[$R$-416]\ * #,##0.0000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-[$R$-416]\ * #,##0.00000_-;\-[$R$-416]\ * #,##0.00000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +267,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -312,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -320,12 +328,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -663,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC4B103-E629-498B-A31B-B855ECF12348}">
   <dimension ref="A6:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>30000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="8" spans="7:11" x14ac:dyDescent="0.25">
@@ -748,6 +757,7 @@
       <c r="I14" t="s">
         <v>54</v>
       </c>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
@@ -780,7 +790,7 @@
       </c>
       <c r="H17" s="13">
         <f>10*(H7/'racional pré def'!K11)</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="I17" t="s">
         <v>61</v>
@@ -889,15 +899,15 @@
       </c>
       <c r="H30" s="6">
         <f>H18*H17*((H9+H11)/60)</f>
-        <v>8039.6699999999992</v>
+        <v>13399.449999999999</v>
       </c>
       <c r="J30" s="5">
         <f>H18*H17*((H10+H11)/60)</f>
-        <v>7034.7112499999994</v>
+        <v>11724.518749999999</v>
       </c>
       <c r="L30" s="5">
         <f>H30-J30</f>
-        <v>1004.9587499999998</v>
+        <v>1674.9312499999996</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -943,17 +953,17 @@
       </c>
       <c r="H33" s="15">
         <f>SUM(H30:H32)</f>
-        <v>64513.908476190474</v>
+        <v>69873.68847619048</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="15">
         <f>SUM(J30:J32)</f>
-        <v>56455.270488095237</v>
+        <v>61145.077988095232</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="15">
         <f>SUM(L30:L32)</f>
-        <v>8058.6379880952409</v>
+        <v>8728.6104880952407</v>
       </c>
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.25">
@@ -991,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911753AC-9533-43E9-9448-6AB317B852D7}">
   <dimension ref="G8:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
versão ajustada do simulador financeiro (excel) com adição da aba melhorias e ajuste na fórmula da metragem
</commit_message>
<xml_diff>
--- a/GuilhermeToledo/SimuladorFinanceiro_v1.xlsx
+++ b/GuilhermeToledo/SimuladorFinanceiro_v1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_toledo_sptech_school/Documents/202501/Pesquisa e Inovação/repositorio_PI/GuilhermeToledo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - SPTech School\202501\Pesquisa e Inovação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{EF76DA37-AE53-42E6-AFF1-46FDB6BE44D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EEDC959-B906-46A0-9A18-3E9E49DD7008}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B035989-0BD9-4495-9C76-7801DFA5D6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2EF024B9-F251-4A5D-B513-02DE12B0E257}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EF024B9-F251-4A5D-B513-02DE12B0E257}"/>
   </bookViews>
   <sheets>
     <sheet name="calc v1" sheetId="1" r:id="rId1"/>
-    <sheet name="racional pré def" sheetId="2" r:id="rId2"/>
-    <sheet name="notas" sheetId="3" r:id="rId3"/>
+    <sheet name="melhorias" sheetId="4" r:id="rId2"/>
+    <sheet name="racional pré def" sheetId="2" r:id="rId3"/>
+    <sheet name="notas" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>metragem área protegida</t>
   </si>
@@ -193,9 +194,6 @@
     <t>litro</t>
   </si>
   <si>
-    <t>bombeiros por 10000 m²</t>
-  </si>
-  <si>
     <t>hora/bombeiro</t>
   </si>
   <si>
@@ -236,18 +234,95 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>10 bombeiros por 10000 m²</t>
+  </si>
+  <si>
+    <t>diretos</t>
+  </si>
+  <si>
+    <t>indiretos</t>
+  </si>
+  <si>
+    <t>desmatamento</t>
+  </si>
+  <si>
+    <t>https://dataserver-coids.inpe.br/queimadas/queimadas/Publicacoes-Impacto/material3os/preco_fogo_diaznepstad.pdf</t>
+  </si>
+  <si>
+    <t>emissão de CO2</t>
+  </si>
+  <si>
+    <t>comorbidades</t>
+  </si>
+  <si>
+    <t>áreas agrícolas?</t>
+  </si>
+  <si>
+    <t>Os prejuízos econômicos associados com a perda de madeira comercializável
+foram estimados multiplicando a área total atingida pelo incêndio florestal pela perda por hectare estimada em Paragominas (US$ 5/ha) em 1998. Ajustado pelo inflação, equivale a 9,87 US$ hoje. Que  equivale a R$57,36/ha. Em termos de m², isso equivale a R$0,005736.</t>
+  </si>
+  <si>
+    <t>Os incêndios que queimaram 2,4 milhões de hectares na Amazônia entre junho e agosto de 2024 emitiram 31,5 milhões de toneladas de CO2 equivalente.</t>
+  </si>
+  <si>
+    <t>CO2 por m²</t>
+  </si>
+  <si>
+    <t>O benefício marginal de redução também pode ser calculado como o imposto necessário para
+reduzir em uma unidade a emissão de CO2, isto é, um preço sombra do carbono21. Os
+valores médios encontrados nesses trabalhos para o benefício marginal variam entre
+US$ 5-10 por tonelada de CO2. Consideramos o valor de US$7.5 por tonelada em 2002. Atualizando o valor para os dias atuais, seriam US$13.37 por tonelada em 2024, que correspondem a R$82,78 por tonelada de CO2.</t>
+  </si>
+  <si>
+    <t>2,4 milhões de hectares queimados emitiram 31,5 milhões de toneladas de CO2, representando 13,125 toneladas de CO2 por hectare. 1 hectare equivale a 10000m². Logo, 1 m² representa 0.0013125 toneladas de CO2.</t>
+  </si>
+  <si>
+    <t>custo da emissão de CO2 por m2</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>quantidade de bombeiros por m²</t>
+  </si>
+  <si>
+    <t>Adicionar temp e umidade como fatores que aceleram a velocidade de expansão do incêndio</t>
+  </si>
+  <si>
+    <t>Adicionar uma tabela no simulador com as pré definicoes</t>
+  </si>
+  <si>
+    <t>Explicar no simulador o racional por tras de cada conta</t>
+  </si>
+  <si>
+    <t>Adicionar a porcentagem de redução de custo para a diferença entre o atual e a solução</t>
+  </si>
+  <si>
+    <t>Adicionar mensagem de alerta caso uma das variáveis esteja faltando</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>Melhorias</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.0000_-;\-[$R$-416]\ * #,##0.0000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-[$R$-416]\ * #,##0.00000_-;\-[$R$-416]\ * #,##0.00000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +342,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -301,7 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -334,7 +417,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -670,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC4B103-E629-498B-A31B-B855ECF12348}">
-  <dimension ref="A6:L38"/>
+  <dimension ref="A6:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +768,7 @@
     <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="7:11" x14ac:dyDescent="0.25">
@@ -712,7 +798,7 @@
         <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="7:11" x14ac:dyDescent="0.25">
@@ -723,18 +809,18 @@
         <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1">
         <v>180</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="7:11" x14ac:dyDescent="0.25">
@@ -751,116 +837,116 @@
         <v>10</v>
       </c>
       <c r="H14" s="12">
-        <f>'racional pré def'!K14</f>
+        <f>'racional pré def'!K9</f>
         <v>1.25</v>
       </c>
       <c r="I14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="16"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="12">
-        <f>'racional pré def'!K9</f>
+        <f>'racional pré def'!K10</f>
         <v>3.4285714285714284</v>
       </c>
       <c r="I15" t="s">
-        <v>57</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H16" s="14">
-        <f>'racional pré def'!K10</f>
+        <f>'racional pré def'!K11</f>
         <v>4.8399999999999997E-3</v>
       </c>
       <c r="I16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="13">
-        <f>10*(H7/'racional pré def'!K11)</f>
+        <f>10*(H7/'racional pré def'!K12)</f>
         <v>50</v>
       </c>
       <c r="I17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="6">
-        <f>'racional pré def'!K12</f>
+        <f>'racional pré def'!K13</f>
         <v>66.997249999999994</v>
       </c>
       <c r="I18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="6">
-        <f>IF(H19 = "sim",'racional pré def'!K13,0)</f>
+        <f>IF(H19 = "sim",'racional pré def'!K14,0)</f>
         <v>14047.619047619048</v>
       </c>
       <c r="I20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G23" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H24" s="6"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G27" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H28" s="3" t="s">
         <v>12</v>
       </c>
@@ -871,26 +957,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="9">
-        <f>IF((H9*60)+(H11*60)*H14&gt;H7,H7,(H9*60)+(H11*60)*H14)</f>
-        <v>17100</v>
+        <f>IF(((H9*60)+(H11*60))*H14&gt;H7,H7,((H9*60)+(H11*60))*H14)</f>
+        <v>18000</v>
       </c>
       <c r="I29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J29" s="9">
-        <f>IF((H10*60)+(H11*60)*H14&gt;H7,H7,(H10*60)+(H11*60)*H14)</f>
-        <v>15300</v>
+        <f>IF(((H10*60)+(H11*60))*H14&gt;H7,H7,((H10*60)+(H11*60))*H14)</f>
+        <v>15750</v>
       </c>
       <c r="K29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="L29" s="9">
+        <f>H29-J29</f>
+        <v>2250</v>
+      </c>
+      <c r="M29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -910,7 +1003,7 @@
         <v>1674.9312499999996</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -919,18 +1012,18 @@
       </c>
       <c r="H31" s="6">
         <f>H15*H29*H16</f>
-        <v>283.76228571428567</v>
+        <v>298.69714285714281</v>
       </c>
       <c r="J31" s="5">
         <f>H15*J29*H16</f>
-        <v>253.89257142857142</v>
+        <v>261.35999999999996</v>
       </c>
       <c r="L31" s="5">
         <f t="shared" ref="L31:L32" si="0">H31-J31</f>
-        <v>29.869714285714252</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>37.337142857142851</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G32" s="1" t="s">
         <v>18</v>
       </c>
@@ -949,21 +1042,21 @@
     </row>
     <row r="33" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G33" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H33" s="15">
         <f>SUM(H30:H32)</f>
-        <v>69873.68847619048</v>
+        <v>69888.623333333337</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="15">
         <f>SUM(J30:J32)</f>
-        <v>61145.077988095232</v>
+        <v>61152.54541666666</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="15">
         <f>SUM(L30:L32)</f>
-        <v>8728.6104880952407</v>
+        <v>8736.0779166666689</v>
       </c>
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.25">
@@ -985,10 +1078,48 @@
     </row>
     <row r="37" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G37" s="3"/>
+      <c r="H37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="38" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G38" s="3" t="s">
-        <v>12</v>
+      <c r="G38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" s="6">
+        <f>H29*'racional pré def'!K17</f>
+        <v>103.24799999999999</v>
+      </c>
+      <c r="J38" s="5">
+        <f>J29*'racional pré def'!K17</f>
+        <v>90.341999999999999</v>
+      </c>
+      <c r="L38" s="5">
+        <f>H38-J38</f>
+        <v>12.905999999999992</v>
+      </c>
+    </row>
+    <row r="39" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H39" s="6">
+        <f>H29*'racional pré def'!K19*'racional pré def'!K18</f>
+        <v>2.5668267187500002</v>
+      </c>
+      <c r="J39" s="5">
+        <f>J29*'racional pré def'!K19*'racional pré def'!K18</f>
+        <v>2.2459733789062502</v>
+      </c>
+      <c r="L39" s="5">
+        <f>H39-J39</f>
+        <v>0.32085333984375008</v>
       </c>
     </row>
   </sheetData>
@@ -998,20 +1129,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29A1392-B542-4C80-9414-F948DE51A3CD}">
+  <dimension ref="B5:C10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911753AC-9533-43E9-9448-6AB317B852D7}">
-  <dimension ref="G8:P14"/>
+  <dimension ref="G8:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="11" max="11" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G8" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="I8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1024,142 +1209,229 @@
     </row>
     <row r="9" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="L9" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K10" s="8">
         <f>24000/7000</f>
         <v>3.4285714285714284</v>
       </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-      <c r="P9" s="1" t="s">
+      <c r="L10" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="10">
-        <v>4.8399999999999997E-3</v>
-      </c>
-      <c r="L10" t="s">
-        <v>50</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="11">
-        <v>10000</v>
+        <v>49</v>
+      </c>
+      <c r="K11" s="10">
+        <v>4.8399999999999997E-3</v>
       </c>
       <c r="L11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="11">
+        <v>10000</v>
+      </c>
+      <c r="L12" t="s">
+        <v>65</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J13" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K13" s="5">
         <f>2679.89/40</f>
         <v>66.997249999999994</v>
       </c>
-      <c r="L12" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12" s="1" t="s">
+      <c r="L13" t="s">
+        <v>51</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G13" s="3" t="s">
+    <row r="14" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K14" s="5">
         <f>(5900000/420)</f>
         <v>14047.619047619048</v>
       </c>
-      <c r="L13" t="s">
-        <v>53</v>
-      </c>
-      <c r="P13" s="1" t="s">
+      <c r="L14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K14" s="8">
-        <v>1.25</v>
-      </c>
-      <c r="L14" t="s">
-        <v>54</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>10</v>
-      </c>
+    <row r="16" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17" s="5">
+        <f>57.36/10000</f>
+        <v>5.7359999999999998E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" s="5">
+        <f>82.78*K19</f>
+        <v>0.10864875</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="16">
+        <f>(31500000/2400000)/10000</f>
+        <v>1.3125000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="7:11" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="K22" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I13" r:id="rId1" display="https://g1.globo.com/sp/sao-paulo/noticia/2024/09/06/com-avanco-das-queimadas-governo-de-sp-libera-r-59-milhoes-para-combate-a-incendios-florestais-com-aeronaves.ghtml" xr:uid="{0E6C05D7-4FBB-44C3-B2BB-B24146BF89C0}"/>
-    <hyperlink ref="I14" r:id="rId2" xr:uid="{A84EB857-86FE-42A6-B4A7-E9AA64DAD431}"/>
-    <hyperlink ref="I12" r:id="rId3" xr:uid="{1EEE96AA-AF67-4757-B12C-AA1A4E14C161}"/>
-    <hyperlink ref="I9" r:id="rId4" xr:uid="{77615B53-3C9F-4821-BD90-7EFF67F5EB92}"/>
-    <hyperlink ref="I11" r:id="rId5" xr:uid="{CC2BB99F-7392-4F66-98C4-F08D091FABE5}"/>
-    <hyperlink ref="I10" r:id="rId6" location=":~:text=J%C3%A1%20para%20a%20categoria%20Residencial,e%20distribui%C3%A7%C3%A3o%20da%20%C3%A1gua%20tratada." xr:uid="{AA5436D9-D730-4003-ACE9-9F26FA66A327}"/>
+    <hyperlink ref="I14" r:id="rId1" display="https://g1.globo.com/sp/sao-paulo/noticia/2024/09/06/com-avanco-das-queimadas-governo-de-sp-libera-r-59-milhoes-para-combate-a-incendios-florestais-com-aeronaves.ghtml" xr:uid="{0E6C05D7-4FBB-44C3-B2BB-B24146BF89C0}"/>
+    <hyperlink ref="I9" r:id="rId2" xr:uid="{A84EB857-86FE-42A6-B4A7-E9AA64DAD431}"/>
+    <hyperlink ref="I13" r:id="rId3" xr:uid="{1EEE96AA-AF67-4757-B12C-AA1A4E14C161}"/>
+    <hyperlink ref="I10" r:id="rId4" xr:uid="{77615B53-3C9F-4821-BD90-7EFF67F5EB92}"/>
+    <hyperlink ref="I12" r:id="rId5" xr:uid="{CC2BB99F-7392-4F66-98C4-F08D091FABE5}"/>
+    <hyperlink ref="I11" r:id="rId6" location=":~:text=J%C3%A1%20para%20a%20categoria%20Residencial,e%20distribui%C3%A7%C3%A3o%20da%20%C3%A1gua%20tratada." xr:uid="{AA5436D9-D730-4003-ACE9-9F26FA66A327}"/>
+    <hyperlink ref="I17" r:id="rId7" xr:uid="{0144C0FF-3A0D-47C3-9F09-4241D0D1D9CB}"/>
+    <hyperlink ref="I18:I20" r:id="rId8" display="https://dataserver-coids.inpe.br/queimadas/queimadas/Publicacoes-Impacto/material3os/preco_fogo_diaznepstad.pdf" xr:uid="{D28F0AAE-BA41-4D0C-9BC7-C626C4E3396A}"/>
+    <hyperlink ref="I21" r:id="rId9" xr:uid="{23E31E48-C77D-4F74-9F99-8765FF6040BF}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B585DECA-C2E9-4378-97B6-86721A3A4AD5}">
   <dimension ref="G10:G18"/>
   <sheetViews>

</xml_diff>